<commit_message>
Add find wiki. Change png and pdf file permissions
</commit_message>
<xml_diff>
--- a/school/files/fall-2020/BUSE-120/module-5/financial_worksheets_module-5.xlsx
+++ b/school/files/fall-2020/BUSE-120/module-5/financial_worksheets_module-5.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393D34DD-6F6E-4895-81D8-B52E1E0130E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEE76A6-C9E1-4EBB-8784-9E312E47E496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="19200" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16530" yWindow="0" windowWidth="21870" windowHeight="16200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="132">
   <si>
     <t>Annual</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>BALANCE SHEET</t>
-  </si>
-  <si>
-    <t>[Enter your name here]</t>
   </si>
   <si>
     <t>Budgeted</t>
@@ -1368,102 +1365,6 @@
   <dxfs count="81">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_)@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <color rgb="FFFF0000"/>
@@ -1591,7 +1492,71 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
@@ -1603,6 +1568,38 @@
       </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_)@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="_)@"/>
@@ -5918,9 +5915,9 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tblSavings" displayName="tblSavings" ref="Q30:S36" totalsRowCount="1">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Savings/Investments" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Savings/Investments" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>tblSavings[[#This Row],[Annual  ]]/12</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5931,9 +5928,9 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tblIncome40" displayName="tblIncome40" ref="B39:D46" totalsRowCount="1">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Income Withholdings" totalsRowLabel=" Total " dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Income Withholdings" totalsRowLabel=" Total " dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Annual  " totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Monthly " totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1">
       <calculatedColumnFormula>tblIncome40[[#This Row],[Annual  ]]/12</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6174,7 +6171,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6201,7 +6198,7 @@
     <row r="2" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2"/>
       <c r="B2" s="138" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -6226,7 +6223,7 @@
     </row>
     <row r="5" spans="1:6" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B5" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="66">
         <f>tblCurrentAssets[[#Totals],[VALUE]]-tblCurrentLiabilities[[#Totals],[AMOUNT]]</f>
@@ -6234,7 +6231,7 @@
       </c>
       <c r="D5" s="45"/>
       <c r="E5" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="66">
         <f>C42-F32</f>
@@ -6268,29 +6265,29 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="134" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="135">
         <v>92</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="136" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" s="137">
         <v>0</v>
@@ -6298,14 +6295,14 @@
     </row>
     <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="134" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="135">
         <v>12287.74</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="136" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" s="137">
         <v>0</v>
@@ -6313,14 +6310,14 @@
     </row>
     <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="134" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="135">
         <v>896</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="136" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" s="137">
         <v>0</v>
@@ -6328,14 +6325,14 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="134" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="135">
         <v>0</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="136" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" s="137">
         <v>0</v>
@@ -6343,14 +6340,14 @@
     </row>
     <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="134" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="135">
         <v>0</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="136" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F14" s="137">
         <v>0</v>
@@ -6358,14 +6355,14 @@
     </row>
     <row r="15" spans="1:6" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="134" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="135">
         <v>8336.58</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="136" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" s="137">
         <v>0</v>
@@ -6373,53 +6370,53 @@
     </row>
     <row r="16" spans="1:6" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="134" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="135">
         <v>4070.66</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="137"/>
     </row>
     <row r="17" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="134" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="135">
         <v>0</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" s="137"/>
     </row>
     <row r="18" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="134" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="135">
         <v>0</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="137"/>
     </row>
     <row r="19" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="134" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="135">
         <v>0</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F19" s="47">
         <f>SUBTOTAL(109,tblCurrentLiabilities[AMOUNT])</f>
@@ -6428,7 +6425,7 @@
     </row>
     <row r="20" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="134" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="135">
         <v>0</v>
@@ -6439,25 +6436,25 @@
     </row>
     <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B21" s="134" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="135"/>
       <c r="D21" s="19"/>
       <c r="E21" s="48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B22" s="134" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="135"/>
       <c r="D22" s="19"/>
       <c r="E22" s="136" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F22" s="137">
         <v>5739</v>
@@ -6465,12 +6462,12 @@
     </row>
     <row r="23" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B23" s="134" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="135"/>
       <c r="D23" s="19"/>
       <c r="E23" s="136" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F23" s="137">
         <v>0</v>
@@ -6478,12 +6475,12 @@
     </row>
     <row r="24" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B24" s="134" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="135"/>
       <c r="D24" s="16"/>
       <c r="E24" s="136" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" s="137">
         <v>0</v>
@@ -6491,14 +6488,14 @@
     </row>
     <row r="25" spans="2:6" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B25" s="132" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="133">
         <f>SUBTOTAL(109,tblCurrentAssets[VALUE])</f>
         <v>25682.98</v>
       </c>
       <c r="E25" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="137"/>
     </row>
@@ -6506,56 +6503,56 @@
       <c r="B26" s="150"/>
       <c r="C26" s="150"/>
       <c r="E26" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" s="137"/>
     </row>
     <row r="27" spans="2:6" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B27" s="48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" s="137"/>
     </row>
     <row r="28" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="136" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="137">
         <v>0</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="137"/>
     </row>
     <row r="29" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="136" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="137">
         <v>0</v>
       </c>
       <c r="E29" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F29" s="137"/>
     </row>
     <row r="30" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="136" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="137">
         <v>0</v>
       </c>
       <c r="E30" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F30" s="47">
         <f>SUBTOTAL(109,tblOtherLiabilities[AMOUNT])</f>
@@ -6574,7 +6571,7 @@
     </row>
     <row r="32" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="136" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C32" s="137">
         <v>2000</v>
@@ -6589,7 +6586,7 @@
     </row>
     <row r="33" spans="2:6" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B33" s="136" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="137">
         <v>0</v>
@@ -6597,7 +6594,7 @@
     </row>
     <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="136" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" s="137">
         <v>600</v>
@@ -6607,7 +6604,7 @@
     </row>
     <row r="35" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="137"/>
       <c r="E35" s="15"/>
@@ -6615,7 +6612,7 @@
     </row>
     <row r="36" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="137"/>
       <c r="E36" s="25"/>
@@ -6623,25 +6620,25 @@
     </row>
     <row r="37" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="137"/>
     </row>
     <row r="38" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="137"/>
     </row>
     <row r="39" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="137"/>
     </row>
     <row r="40" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C40" s="65">
         <f>SUBTOTAL(109,tblOtherAssets[VALUE])</f>
@@ -6664,7 +6661,7 @@
     <row r="43" spans="2:6" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="146" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -6694,8 +6691,8 @@
   </sheetPr>
   <dimension ref="A1:AJ61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="R35" sqref="R35"/>
+    <sheetView showGridLines="0" topLeftCell="P7" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6718,7 +6715,7 @@
     <row r="1" spans="1:36" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1"/>
       <c r="B1" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
@@ -6753,7 +6750,7 @@
     <row r="2" spans="1:36" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A2"/>
       <c r="B2" s="138" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -6844,13 +6841,13 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="L6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="Q6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -7302,7 +7299,7 @@
     </row>
     <row r="30" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>27</v>
@@ -7311,7 +7308,7 @@
         <v>26</v>
       </c>
       <c r="E30" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G30" s="58" t="s">
         <v>29</v>
@@ -7323,7 +7320,7 @@
         <v>26</v>
       </c>
       <c r="J30" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L30" s="58" t="s">
         <v>9</v>
@@ -7335,10 +7332,10 @@
         <v>26</v>
       </c>
       <c r="O30" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q30" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R30" s="7" t="s">
         <v>27</v>
@@ -7347,12 +7344,12 @@
         <v>26</v>
       </c>
       <c r="T30" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="57">
         <v>7524</v>
@@ -7428,7 +7425,7 @@
       </c>
       <c r="F32" s="36"/>
       <c r="G32" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H32" s="57">
         <v>400</v>
@@ -7458,7 +7455,7 @@
       </c>
       <c r="P32" s="36"/>
       <c r="Q32" s="56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R32" s="57">
         <v>0</v>
@@ -7474,7 +7471,7 @@
     </row>
     <row r="33" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="35">
@@ -7517,7 +7514,7 @@
       </c>
       <c r="P33" s="36"/>
       <c r="Q33" s="56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R33" s="57">
         <v>1440</v>
@@ -7533,7 +7530,7 @@
     </row>
     <row r="34" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="57"/>
       <c r="D34" s="35">
@@ -7576,7 +7573,7 @@
       </c>
       <c r="P34" s="36"/>
       <c r="Q34" s="56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="R34" s="57">
         <v>600</v>
@@ -7592,7 +7589,7 @@
     </row>
     <row r="35" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="57"/>
       <c r="D35" s="35">
@@ -7605,7 +7602,7 @@
       </c>
       <c r="F35" s="36"/>
       <c r="G35" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H35" s="57">
         <v>400</v>
@@ -7635,7 +7632,7 @@
       </c>
       <c r="P35" s="36"/>
       <c r="Q35" s="56" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R35" s="57"/>
       <c r="S35" s="35">
@@ -7649,7 +7646,7 @@
     </row>
     <row r="36" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="57"/>
       <c r="D36" s="35">
@@ -7662,7 +7659,7 @@
       </c>
       <c r="F36" s="36"/>
       <c r="G36" s="56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H36" s="57">
         <v>0</v>
@@ -7709,7 +7706,7 @@
     </row>
     <row r="37" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="35">
         <f>SUBTOTAL(109,tblIncome[[Annual  ]])</f>
@@ -7765,7 +7762,7 @@
       <c r="E38" s="36"/>
       <c r="F38" s="36"/>
       <c r="G38" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H38" s="57">
         <v>0</v>
@@ -7795,7 +7792,7 @@
       </c>
       <c r="P38" s="36"/>
       <c r="Q38" s="59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R38" s="39" t="s">
         <v>0</v>
@@ -7804,12 +7801,12 @@
         <v>1</v>
       </c>
       <c r="T38" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="38" t="s">
         <v>27</v>
@@ -7818,7 +7815,7 @@
         <v>26</v>
       </c>
       <c r="E39" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39" s="36"/>
       <c r="G39" s="56" t="s">
@@ -7837,7 +7834,7 @@
       </c>
       <c r="K39" s="36"/>
       <c r="L39" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M39" s="57">
         <v>150</v>
@@ -7852,7 +7849,7 @@
       </c>
       <c r="P39" s="36"/>
       <c r="Q39" s="61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R39" s="41">
         <f>M51</f>
@@ -7869,7 +7866,7 @@
     </row>
     <row r="40" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="57">
         <v>0</v>
@@ -7899,7 +7896,7 @@
       </c>
       <c r="K40" s="36"/>
       <c r="L40" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M40" s="57"/>
       <c r="N40" s="35">
@@ -7912,7 +7909,7 @@
       </c>
       <c r="P40" s="36"/>
       <c r="Q40" s="61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R40" s="41">
         <f>R36</f>
@@ -7929,7 +7926,7 @@
     </row>
     <row r="41" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="57">
         <v>0</v>
@@ -7944,7 +7941,7 @@
       </c>
       <c r="F41" s="36"/>
       <c r="G41" s="56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H41" s="57">
         <v>1440</v>
@@ -7959,7 +7956,7 @@
       </c>
       <c r="K41" s="36"/>
       <c r="L41" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M41" s="57"/>
       <c r="N41" s="35">
@@ -7972,7 +7969,7 @@
       </c>
       <c r="P41" s="36"/>
       <c r="Q41" s="60" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R41" s="42">
         <f>R39-R40</f>
@@ -7989,7 +7986,7 @@
     </row>
     <row r="42" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="57">
         <v>0</v>
@@ -8004,7 +8001,7 @@
       </c>
       <c r="F42" s="36"/>
       <c r="G42" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H42" s="57"/>
       <c r="I42" s="74">
@@ -8017,7 +8014,7 @@
       </c>
       <c r="K42" s="36"/>
       <c r="L42" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M42" s="57"/>
       <c r="N42" s="35">
@@ -8036,7 +8033,7 @@
     </row>
     <row r="43" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" s="57">
         <v>0</v>
@@ -8051,7 +8048,7 @@
       </c>
       <c r="F43" s="36"/>
       <c r="G43" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H43" s="57"/>
       <c r="I43" s="74">
@@ -8064,7 +8061,7 @@
       </c>
       <c r="K43" s="36"/>
       <c r="L43" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M43" s="57"/>
       <c r="N43" s="35">
@@ -8083,7 +8080,7 @@
     </row>
     <row r="44" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" s="57"/>
       <c r="D44" s="35">
@@ -8096,7 +8093,7 @@
       </c>
       <c r="F44" s="36"/>
       <c r="G44" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H44" s="57"/>
       <c r="I44" s="74">
@@ -8109,7 +8106,7 @@
       </c>
       <c r="K44" s="36"/>
       <c r="L44" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M44" s="57"/>
       <c r="N44" s="35">
@@ -8128,7 +8125,7 @@
     </row>
     <row r="45" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="57"/>
       <c r="D45" s="35">
@@ -8141,7 +8138,7 @@
       </c>
       <c r="F45" s="36"/>
       <c r="G45" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H45" s="57"/>
       <c r="I45" s="74">
@@ -8154,7 +8151,7 @@
       </c>
       <c r="K45" s="36"/>
       <c r="L45" s="58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M45" s="35">
         <f>SUBTOTAL(109,tblDiscretionary[[Annual  ]])</f>
@@ -8176,7 +8173,7 @@
     </row>
     <row r="46" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C46" s="35">
         <f>SUBTOTAL(109,tblIncome40[[Annual  ]])</f>
@@ -8192,7 +8189,7 @@
       </c>
       <c r="F46" s="36"/>
       <c r="G46" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H46" s="57"/>
       <c r="I46" s="74">
@@ -8220,7 +8217,7 @@
       <c r="E47" s="36"/>
       <c r="F47" s="36"/>
       <c r="G47" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H47" s="57"/>
       <c r="I47" s="74">
@@ -8233,7 +8230,7 @@
       </c>
       <c r="K47" s="36"/>
       <c r="L47" s="59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M47" s="39" t="s">
         <v>0</v>
@@ -8242,7 +8239,7 @@
         <v>1</v>
       </c>
       <c r="O47" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P47" s="36"/>
       <c r="Q47" s="36"/>
@@ -8252,7 +8249,7 @@
     </row>
     <row r="48" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" s="39" t="s">
         <v>0</v>
@@ -8261,11 +8258,11 @@
         <v>1</v>
       </c>
       <c r="E48" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F48" s="36"/>
       <c r="G48" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H48" s="57"/>
       <c r="I48" s="74">
@@ -8278,7 +8275,7 @@
       </c>
       <c r="K48" s="36"/>
       <c r="L48" s="62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M48" s="41">
         <f>C51</f>
@@ -8300,7 +8297,7 @@
     </row>
     <row r="49" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" s="64">
         <f>tblIncome[[#Totals],[Annual  ]]</f>
@@ -8316,7 +8313,7 @@
       </c>
       <c r="F49" s="36"/>
       <c r="G49" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H49" s="57"/>
       <c r="I49" s="74">
@@ -8329,7 +8326,7 @@
       </c>
       <c r="K49" s="36"/>
       <c r="L49" s="62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M49" s="41">
         <f>tblExpenses[[#Totals],[Annual  ]]</f>
@@ -8351,7 +8348,7 @@
     </row>
     <row r="50" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="64">
         <f>tblIncome40[[#Totals],[Annual  ]]</f>
@@ -8367,7 +8364,7 @@
       </c>
       <c r="F50" s="36"/>
       <c r="G50" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H50" s="57"/>
       <c r="I50" s="74">
@@ -8380,7 +8377,7 @@
       </c>
       <c r="K50" s="36"/>
       <c r="L50" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M50" s="41">
         <f>tblDiscretionary[[#Totals],[Annual  ]]</f>
@@ -8402,7 +8399,7 @@
     </row>
     <row r="51" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51" s="42">
         <f>C49-C50</f>
@@ -8418,7 +8415,7 @@
       </c>
       <c r="F51" s="36"/>
       <c r="G51" s="58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H51" s="35">
         <f>SUM(tblExpenses[[Annual  ]])</f>
@@ -8434,7 +8431,7 @@
       </c>
       <c r="K51" s="36"/>
       <c r="L51" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M51" s="42">
         <f>M48-M49-M50</f>
@@ -8493,7 +8490,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8507,14 +8504,14 @@
     <row r="1" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1"/>
       <c r="B1" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2"/>
       <c r="B2" s="138" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="26"/>
     </row>
@@ -8531,19 +8528,19 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="155" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="155"/>
     </row>
     <row r="6" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="154" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="154"/>
     </row>
     <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="126" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="139">
         <v>20000</v>
@@ -8551,7 +8548,7 @@
     </row>
     <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="127" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="140">
         <v>0.05</v>
@@ -8559,19 +8556,19 @@
     </row>
     <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="126" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="141">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="128" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="129">
         <f>IF(C9=0,"",(C7*(C8/12)/(((1+(C8/12))^C9)-1)))</f>
-        <v>294.09133954688417</v>
+        <v>199.34484810480592</v>
       </c>
     </row>
   </sheetData>
@@ -8592,9 +8589,9 @@
   </sheetPr>
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8612,7 +8609,7 @@
     <row r="1" spans="1:9" s="16" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1"/>
       <c r="B1" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
@@ -8622,7 +8619,7 @@
     <row r="2" spans="1:9" s="16" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2"/>
       <c r="B2" s="138" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -8632,7 +8629,7 @@
     <row r="3" spans="1:9" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="138" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
@@ -8647,27 +8644,27 @@
         <v>20</v>
       </c>
       <c r="D5" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="G5" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="67" t="s">
-        <v>39</v>
-      </c>
       <c r="H5" s="67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="77" t="str">
         <f>'Cash Flow'!B31</f>
@@ -8677,7 +8674,9 @@
         <f>'Cash Flow'!D31</f>
         <v>627</v>
       </c>
-      <c r="E6" s="142"/>
+      <c r="E6" s="142">
+        <v>627</v>
+      </c>
       <c r="F6" s="142"/>
       <c r="G6" s="84" t="str">
         <f>IF(F6=0,"",F6-E6)</f>
@@ -8691,7 +8690,7 @@
     </row>
     <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="77" t="str">
         <f>'Cash Flow'!B32</f>
@@ -8701,7 +8700,9 @@
         <f>'Cash Flow'!D32</f>
         <v>0</v>
       </c>
-      <c r="E7" s="142"/>
+      <c r="E7" s="142">
+        <v>0</v>
+      </c>
       <c r="F7" s="142"/>
       <c r="G7" s="84" t="str">
         <f t="shared" ref="G7:G62" si="0">IF(F7=0,"",F7-E7)</f>
@@ -8715,7 +8716,7 @@
     </row>
     <row r="8" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="77" t="str">
         <f>'Cash Flow'!B33</f>
@@ -8725,7 +8726,9 @@
         <f>'Cash Flow'!D33</f>
         <v>0</v>
       </c>
-      <c r="E8" s="142"/>
+      <c r="E8" s="142">
+        <v>0</v>
+      </c>
       <c r="F8" s="142"/>
       <c r="G8" s="84" t="str">
         <f t="shared" si="0"/>
@@ -8739,7 +8742,7 @@
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="77" t="str">
         <f>'Cash Flow'!B34</f>
@@ -8749,7 +8752,9 @@
         <f>'Cash Flow'!D34</f>
         <v>0</v>
       </c>
-      <c r="E9" s="142"/>
+      <c r="E9" s="142">
+        <v>0</v>
+      </c>
       <c r="F9" s="142"/>
       <c r="G9" s="84" t="str">
         <f t="shared" si="0"/>
@@ -8763,7 +8768,7 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="77" t="str">
         <f>'Cash Flow'!B35</f>
@@ -8773,7 +8778,9 @@
         <f>'Cash Flow'!D35</f>
         <v>0</v>
       </c>
-      <c r="E10" s="142"/>
+      <c r="E10" s="142">
+        <v>0</v>
+      </c>
       <c r="F10" s="142"/>
       <c r="G10" s="84" t="str">
         <f t="shared" si="0"/>
@@ -8787,7 +8794,7 @@
     </row>
     <row r="11" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="77" t="str">
         <f>'Cash Flow'!B36</f>
@@ -8797,7 +8804,9 @@
         <f>'Cash Flow'!D36</f>
         <v>0</v>
       </c>
-      <c r="E11" s="142"/>
+      <c r="E11" s="142">
+        <v>0</v>
+      </c>
       <c r="F11" s="142"/>
       <c r="G11" s="84" t="str">
         <f t="shared" si="0"/>
@@ -8812,7 +8821,7 @@
     <row r="12" spans="1:9" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="79"/>
       <c r="C12" s="80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="81">
         <f>SUM(D6:D11)</f>
@@ -8820,7 +8829,7 @@
       </c>
       <c r="E12" s="81">
         <f t="shared" ref="E12:F12" si="2">SUM(E6:E11)</f>
-        <v>0</v>
+        <v>627</v>
       </c>
       <c r="F12" s="81">
         <f t="shared" si="2"/>
@@ -8838,7 +8847,7 @@
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="86" t="str">
         <f>'Cash Flow'!B40</f>
@@ -8848,7 +8857,9 @@
         <f>'Cash Flow'!D40</f>
         <v>0</v>
       </c>
-      <c r="E13" s="142"/>
+      <c r="E13" s="142">
+        <v>0</v>
+      </c>
       <c r="F13" s="142"/>
       <c r="G13" s="88" t="str">
         <f t="shared" si="0"/>
@@ -8862,7 +8873,7 @@
     </row>
     <row r="14" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="86" t="str">
         <f>'Cash Flow'!B41</f>
@@ -8872,7 +8883,9 @@
         <f>'Cash Flow'!D41</f>
         <v>0</v>
       </c>
-      <c r="E14" s="142"/>
+      <c r="E14" s="142">
+        <v>0</v>
+      </c>
       <c r="F14" s="142"/>
       <c r="G14" s="88" t="str">
         <f t="shared" si="0"/>
@@ -8886,7 +8899,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="86" t="str">
         <f>'Cash Flow'!B42</f>
@@ -8896,7 +8909,9 @@
         <f>'Cash Flow'!D42</f>
         <v>0</v>
       </c>
-      <c r="E15" s="142"/>
+      <c r="E15" s="142">
+        <v>0</v>
+      </c>
       <c r="F15" s="142"/>
       <c r="G15" s="88" t="str">
         <f t="shared" si="0"/>
@@ -8910,7 +8925,7 @@
     </row>
     <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="86" t="str">
         <f>'Cash Flow'!B43</f>
@@ -8920,7 +8935,9 @@
         <f>'Cash Flow'!D43</f>
         <v>0</v>
       </c>
-      <c r="E16" s="142"/>
+      <c r="E16" s="142">
+        <v>0</v>
+      </c>
       <c r="F16" s="142"/>
       <c r="G16" s="88" t="str">
         <f t="shared" si="0"/>
@@ -8934,7 +8951,7 @@
     </row>
     <row r="17" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="86" t="str">
         <f>'Cash Flow'!B44</f>
@@ -8944,7 +8961,9 @@
         <f>'Cash Flow'!D44</f>
         <v>0</v>
       </c>
-      <c r="E17" s="142"/>
+      <c r="E17" s="142">
+        <v>0</v>
+      </c>
       <c r="F17" s="142"/>
       <c r="G17" s="88" t="str">
         <f t="shared" si="0"/>
@@ -8958,7 +8977,7 @@
     </row>
     <row r="18" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="86" t="str">
         <f>'Cash Flow'!B45</f>
@@ -8968,7 +8987,9 @@
         <f>'Cash Flow'!D45</f>
         <v>0</v>
       </c>
-      <c r="E18" s="142"/>
+      <c r="E18" s="142">
+        <v>0</v>
+      </c>
       <c r="F18" s="142"/>
       <c r="G18" s="88" t="str">
         <f t="shared" si="0"/>
@@ -8983,7 +9004,7 @@
     <row r="19" spans="2:9" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="90"/>
       <c r="C19" s="91" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="92">
         <f>D12-SUM(D13:D18)</f>
@@ -8991,7 +9012,7 @@
       </c>
       <c r="E19" s="92">
         <f t="shared" ref="E19:F19" si="3">E12-SUM(E13:E18)</f>
-        <v>0</v>
+        <v>627</v>
       </c>
       <c r="F19" s="92">
         <f t="shared" si="3"/>
@@ -9019,7 +9040,9 @@
         <f>'Cash Flow'!I31</f>
         <v>0</v>
       </c>
-      <c r="E20" s="142"/>
+      <c r="E20" s="142">
+        <v>0</v>
+      </c>
       <c r="F20" s="142"/>
       <c r="G20" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9043,7 +9066,9 @@
         <f>'Cash Flow'!I32</f>
         <v>33.333333333333336</v>
       </c>
-      <c r="E21" s="142"/>
+      <c r="E21" s="142">
+        <v>33</v>
+      </c>
       <c r="F21" s="142"/>
       <c r="G21" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9067,7 +9092,9 @@
         <f>'Cash Flow'!I33</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="E22" s="142"/>
+      <c r="E22" s="142">
+        <v>40</v>
+      </c>
       <c r="F22" s="142"/>
       <c r="G22" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9091,7 +9118,9 @@
         <f>'Cash Flow'!I34</f>
         <v>0</v>
       </c>
-      <c r="E23" s="142"/>
+      <c r="E23" s="142">
+        <v>0</v>
+      </c>
       <c r="F23" s="142"/>
       <c r="G23" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9115,7 +9144,9 @@
         <f>'Cash Flow'!I35</f>
         <v>33.333333333333336</v>
       </c>
-      <c r="E24" s="142"/>
+      <c r="E24" s="142">
+        <v>33</v>
+      </c>
       <c r="F24" s="142"/>
       <c r="G24" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9139,7 +9170,9 @@
         <f>'Cash Flow'!I36</f>
         <v>0</v>
       </c>
-      <c r="E25" s="142"/>
+      <c r="E25" s="142">
+        <v>0</v>
+      </c>
       <c r="F25" s="142"/>
       <c r="G25" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9163,7 +9196,9 @@
         <f>'Cash Flow'!I37</f>
         <v>30</v>
       </c>
-      <c r="E26" s="142"/>
+      <c r="E26" s="142">
+        <v>30</v>
+      </c>
       <c r="F26" s="142"/>
       <c r="G26" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9187,7 +9222,9 @@
         <f>'Cash Flow'!I38</f>
         <v>0</v>
       </c>
-      <c r="E27" s="142"/>
+      <c r="E27" s="142">
+        <v>0</v>
+      </c>
       <c r="F27" s="142"/>
       <c r="G27" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9211,7 +9248,9 @@
         <f>'Cash Flow'!I39</f>
         <v>0</v>
       </c>
-      <c r="E28" s="142"/>
+      <c r="E28" s="142">
+        <v>0</v>
+      </c>
       <c r="F28" s="142"/>
       <c r="G28" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9235,7 +9274,9 @@
         <f>'Cash Flow'!I40</f>
         <v>0</v>
       </c>
-      <c r="E29" s="142"/>
+      <c r="E29" s="142">
+        <v>0</v>
+      </c>
       <c r="F29" s="142"/>
       <c r="G29" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9259,7 +9300,9 @@
         <f>'Cash Flow'!I41</f>
         <v>120</v>
       </c>
-      <c r="E30" s="142"/>
+      <c r="E30" s="142">
+        <v>120</v>
+      </c>
       <c r="F30" s="142"/>
       <c r="G30" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9283,7 +9326,9 @@
         <f>'Cash Flow'!I42</f>
         <v>0</v>
       </c>
-      <c r="E31" s="142"/>
+      <c r="E31" s="142">
+        <v>0</v>
+      </c>
       <c r="F31" s="142"/>
       <c r="G31" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9307,7 +9352,9 @@
         <f>'Cash Flow'!I43</f>
         <v>0</v>
       </c>
-      <c r="E32" s="142"/>
+      <c r="E32" s="142">
+        <v>0</v>
+      </c>
       <c r="F32" s="142"/>
       <c r="G32" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9331,7 +9378,9 @@
         <f>'Cash Flow'!I44</f>
         <v>0</v>
       </c>
-      <c r="E33" s="142"/>
+      <c r="E33" s="142">
+        <v>0</v>
+      </c>
       <c r="F33" s="142"/>
       <c r="G33" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9355,7 +9404,9 @@
         <f>'Cash Flow'!I45</f>
         <v>0</v>
       </c>
-      <c r="E34" s="142"/>
+      <c r="E34" s="142">
+        <v>0</v>
+      </c>
       <c r="F34" s="142"/>
       <c r="G34" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9379,7 +9430,9 @@
         <f>'Cash Flow'!I46</f>
         <v>0</v>
       </c>
-      <c r="E35" s="142"/>
+      <c r="E35" s="142">
+        <v>0</v>
+      </c>
       <c r="F35" s="142"/>
       <c r="G35" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9403,7 +9456,9 @@
         <f>'Cash Flow'!I47</f>
         <v>0</v>
       </c>
-      <c r="E36" s="142"/>
+      <c r="E36" s="142">
+        <v>0</v>
+      </c>
       <c r="F36" s="142"/>
       <c r="G36" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9427,7 +9482,9 @@
         <f>'Cash Flow'!I48</f>
         <v>0</v>
       </c>
-      <c r="E37" s="142"/>
+      <c r="E37" s="142">
+        <v>0</v>
+      </c>
       <c r="F37" s="142"/>
       <c r="G37" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9451,7 +9508,9 @@
         <f>'Cash Flow'!I49</f>
         <v>0</v>
       </c>
-      <c r="E38" s="142"/>
+      <c r="E38" s="142">
+        <v>0</v>
+      </c>
       <c r="F38" s="142"/>
       <c r="G38" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9475,7 +9534,9 @@
         <f>'Cash Flow'!I50</f>
         <v>0</v>
       </c>
-      <c r="E39" s="142"/>
+      <c r="E39" s="142">
+        <v>0</v>
+      </c>
       <c r="F39" s="142"/>
       <c r="G39" s="97" t="str">
         <f t="shared" si="0"/>
@@ -9490,7 +9551,7 @@
     <row r="40" spans="2:9" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="99"/>
       <c r="C40" s="100" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D40" s="101">
         <f>SUM(D20:D39)</f>
@@ -9498,7 +9559,7 @@
       </c>
       <c r="E40" s="101">
         <f t="shared" ref="E40:F40" si="4">SUM(E20:E39)</f>
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="F40" s="101">
         <f t="shared" si="4"/>
@@ -9526,7 +9587,9 @@
         <f>'Cash Flow'!N31</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="E41" s="142"/>
+      <c r="E41" s="142">
+        <v>20</v>
+      </c>
       <c r="F41" s="142"/>
       <c r="G41" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9550,7 +9613,9 @@
         <f>'Cash Flow'!N32</f>
         <v>0</v>
       </c>
-      <c r="E42" s="142"/>
+      <c r="E42" s="142">
+        <v>0</v>
+      </c>
       <c r="F42" s="142"/>
       <c r="G42" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9574,7 +9639,9 @@
         <f>'Cash Flow'!N33</f>
         <v>0</v>
       </c>
-      <c r="E43" s="142"/>
+      <c r="E43" s="142">
+        <v>0</v>
+      </c>
       <c r="F43" s="142"/>
       <c r="G43" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9598,7 +9665,9 @@
         <f>'Cash Flow'!N34</f>
         <v>50</v>
       </c>
-      <c r="E44" s="142"/>
+      <c r="E44" s="142">
+        <v>0</v>
+      </c>
       <c r="F44" s="142"/>
       <c r="G44" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9622,7 +9691,9 @@
         <f>'Cash Flow'!N35</f>
         <v>20</v>
       </c>
-      <c r="E45" s="142"/>
+      <c r="E45" s="142">
+        <v>20</v>
+      </c>
       <c r="F45" s="142"/>
       <c r="G45" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9646,7 +9717,9 @@
         <f>'Cash Flow'!N36</f>
         <v>0</v>
       </c>
-      <c r="E46" s="142"/>
+      <c r="E46" s="142">
+        <v>0</v>
+      </c>
       <c r="F46" s="142"/>
       <c r="G46" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9670,7 +9743,9 @@
         <f>'Cash Flow'!N37</f>
         <v>0</v>
       </c>
-      <c r="E47" s="142"/>
+      <c r="E47" s="142">
+        <v>0</v>
+      </c>
       <c r="F47" s="142"/>
       <c r="G47" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9694,7 +9769,9 @@
         <f>'Cash Flow'!N38</f>
         <v>0</v>
       </c>
-      <c r="E48" s="142"/>
+      <c r="E48" s="142">
+        <v>0</v>
+      </c>
       <c r="F48" s="142"/>
       <c r="G48" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9718,7 +9795,9 @@
         <f>'Cash Flow'!N39</f>
         <v>12.5</v>
       </c>
-      <c r="E49" s="142"/>
+      <c r="E49" s="142">
+        <v>13</v>
+      </c>
       <c r="F49" s="142"/>
       <c r="G49" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9742,7 +9821,9 @@
         <f>'Cash Flow'!N40</f>
         <v>0</v>
       </c>
-      <c r="E50" s="142"/>
+      <c r="E50" s="142">
+        <v>0</v>
+      </c>
       <c r="F50" s="142"/>
       <c r="G50" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9766,7 +9847,9 @@
         <f>'Cash Flow'!N41</f>
         <v>0</v>
       </c>
-      <c r="E51" s="142"/>
+      <c r="E51" s="142">
+        <v>0</v>
+      </c>
       <c r="F51" s="142"/>
       <c r="G51" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9790,7 +9873,9 @@
         <f>'Cash Flow'!N42</f>
         <v>0</v>
       </c>
-      <c r="E52" s="142"/>
+      <c r="E52" s="142">
+        <v>0</v>
+      </c>
       <c r="F52" s="142"/>
       <c r="G52" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9814,7 +9899,9 @@
         <f>'Cash Flow'!N43</f>
         <v>0</v>
       </c>
-      <c r="E53" s="142"/>
+      <c r="E53" s="142">
+        <v>0</v>
+      </c>
       <c r="F53" s="142"/>
       <c r="G53" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9838,7 +9925,9 @@
         <f>'Cash Flow'!N44</f>
         <v>0</v>
       </c>
-      <c r="E54" s="142"/>
+      <c r="E54" s="142">
+        <v>0</v>
+      </c>
       <c r="F54" s="142"/>
       <c r="G54" s="106" t="str">
         <f t="shared" si="0"/>
@@ -9853,7 +9942,7 @@
     <row r="55" spans="2:9" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="108"/>
       <c r="C55" s="109" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D55" s="110">
         <f>SUM(D41:D54)</f>
@@ -9861,7 +9950,7 @@
       </c>
       <c r="E55" s="110">
         <f t="shared" ref="E55:F55" si="5">SUM(E41:E54)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="F55" s="110">
         <f t="shared" si="5"/>
@@ -9889,7 +9978,9 @@
         <f>'Cash Flow'!S31</f>
         <v>100</v>
       </c>
-      <c r="E56" s="142"/>
+      <c r="E56" s="142">
+        <v>50</v>
+      </c>
       <c r="F56" s="142"/>
       <c r="G56" s="113" t="str">
         <f t="shared" si="0"/>
@@ -9913,7 +10004,9 @@
         <f>'Cash Flow'!S32</f>
         <v>0</v>
       </c>
-      <c r="E57" s="142"/>
+      <c r="E57" s="142">
+        <v>0</v>
+      </c>
       <c r="F57" s="142"/>
       <c r="G57" s="113" t="str">
         <f t="shared" si="0"/>
@@ -9937,7 +10030,9 @@
         <f>'Cash Flow'!S33</f>
         <v>120</v>
       </c>
-      <c r="E58" s="142"/>
+      <c r="E58" s="142">
+        <v>50</v>
+      </c>
       <c r="F58" s="142"/>
       <c r="G58" s="113" t="str">
         <f t="shared" si="0"/>
@@ -9961,7 +10056,9 @@
         <f>'Cash Flow'!S34</f>
         <v>50</v>
       </c>
-      <c r="E59" s="142"/>
+      <c r="E59" s="142">
+        <v>20</v>
+      </c>
       <c r="F59" s="142"/>
       <c r="G59" s="113" t="str">
         <f t="shared" si="0"/>
@@ -9985,7 +10082,9 @@
         <f>'Cash Flow'!S35</f>
         <v>0</v>
       </c>
-      <c r="E60" s="142"/>
+      <c r="E60" s="142">
+        <v>200</v>
+      </c>
       <c r="F60" s="142"/>
       <c r="G60" s="113" t="str">
         <f t="shared" si="0"/>
@@ -10000,7 +10099,7 @@
     <row r="61" spans="2:9" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="115"/>
       <c r="C61" s="116" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D61" s="117">
         <f>SUM(D56:D60)</f>
@@ -10008,7 +10107,7 @@
       </c>
       <c r="E61" s="117">
         <f t="shared" ref="E61:F61" si="6">SUM(E56:E60)</f>
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="F61" s="117">
         <f t="shared" si="6"/>
@@ -10027,7 +10126,7 @@
     <row r="62" spans="2:9" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="120"/>
       <c r="C62" s="121" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D62" s="122">
         <f>D19-D40-D55-D61</f>
@@ -10035,7 +10134,7 @@
       </c>
       <c r="E62" s="122">
         <f t="shared" ref="E62:F62" si="7">E19-E40-E55-E61</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F62" s="122">
         <f t="shared" si="7"/>
@@ -10126,7 +10225,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="H6:H62">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
       <formula>-0.05</formula>
       <formula>0.05</formula>
     </cfRule>

</xml_diff>